<commit_message>
Enhanced the logic for the EventCompile function regarding variable consistency across input conditions.
</commit_message>
<xml_diff>
--- a/ExampleFiles/Event Compile/ExampleOutput/Events_By_Subject.xlsx
+++ b/ExampleFiles/Event Compile/ExampleOutput/Events_By_Subject.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>10.7466118</v>
+        <v>84.3212552</v>
       </c>
       <c r="F2" t="n">
-        <v>1.850743445960936</v>
+        <v>0.8325301005149038</v>
       </c>
       <c r="G2" t="n">
-        <v>-3.0311946</v>
+        <v>55.6811798</v>
       </c>
       <c r="H2" t="n">
-        <v>1.436744653015921</v>
+        <v>0.4847822359189321</v>
       </c>
     </row>
     <row r="3">
@@ -506,7 +506,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -604,16 +604,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>10.306607</v>
+        <v>85.285994</v>
       </c>
       <c r="F5" t="n">
-        <v>1.38343916754471</v>
+        <v>0.7120568096454086</v>
       </c>
       <c r="G5" t="n">
-        <v>-6.430931599999999</v>
+        <v>52.0624512</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8185719096782152</v>
+        <v>0.3091264905506488</v>
       </c>
     </row>
     <row r="6">
@@ -624,7 +624,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -722,16 +722,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>10.9731058</v>
+        <v>87.0443724</v>
       </c>
       <c r="F8" t="n">
-        <v>1.123356858782711</v>
+        <v>0.7722442340152744</v>
       </c>
       <c r="G8" t="n">
-        <v>-7.2956164</v>
+        <v>53.03607459999999</v>
       </c>
       <c r="H8" t="n">
-        <v>0.625493482883267</v>
+        <v>0.432800465373872</v>
       </c>
     </row>
     <row r="9">
@@ -742,7 +742,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -784,7 +784,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -839,21 +839,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E11" t="n">
+        <v>-1.0084284</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3183120638578438</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.3984804</v>
+        <v>-18.5875616</v>
       </c>
       <c r="H11" t="n">
-        <v>0.07220288671957646</v>
+        <v>0.7004253333044419</v>
       </c>
     </row>
     <row r="12">
@@ -864,7 +860,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -906,7 +902,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -948,7 +944,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -961,21 +957,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E14" t="n">
+        <v>12.1551704</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9567180811540255</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.5618934</v>
+        <v>-2.2864472</v>
       </c>
       <c r="H14" t="n">
-        <v>0.03363609307039086</v>
+        <v>0.5347939563837274</v>
       </c>
     </row>
     <row r="15">
@@ -986,7 +978,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1028,7 +1020,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1070,7 +1062,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1083,21 +1075,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E17" t="n">
+        <v>-1.3741346</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.6461043890538433</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.3727668</v>
+        <v>-14.7271458</v>
       </c>
       <c r="H17" t="n">
-        <v>0.05761839744873159</v>
+        <v>5.890145025697462</v>
       </c>
     </row>
     <row r="18">
@@ -1108,7 +1096,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1150,7 +1138,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1192,7 +1180,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1206,16 +1194,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.1506864</v>
+        <v>12.9505352</v>
       </c>
       <c r="F20" t="n">
-        <v>0.07781861838814669</v>
+        <v>9.889571093040029</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.6387319999999999</v>
+        <v>-15.5657846</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1343049492565334</v>
+        <v>11.75479988593403</v>
       </c>
     </row>
     <row r="21">
@@ -1226,7 +1214,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1239,11 +1227,15 @@
           <t>Event 2</t>
         </is>
       </c>
-      <c r="E21" t="n">
-        <v>3.0633316</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.4222676215830904</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1264,7 +1256,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1306,7 +1298,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1320,16 +1312,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.0817206</v>
+        <v>2.7868004</v>
       </c>
       <c r="F23" t="n">
-        <v>0.01152908108393726</v>
+        <v>1.076501950623147</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.5872968000000001</v>
+        <v>-34.337238</v>
       </c>
       <c r="H23" t="n">
-        <v>0.03483551402462724</v>
+        <v>1.757966444595801</v>
       </c>
     </row>
     <row r="24">
@@ -1340,7 +1332,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1354,16 +1346,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3.8510572</v>
+        <v>11.3497572</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1770348084049012</v>
+        <v>1.56200346401452</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.2563444</v>
+        <v>-3.7141776</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1603218457710614</v>
+        <v>1.08491076162984</v>
       </c>
     </row>
     <row r="25">
@@ -1374,7 +1366,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1416,7 +1408,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1430,16 +1422,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.2295378</v>
+        <v>13.301173</v>
       </c>
       <c r="F26" t="n">
-        <v>0.03968428710409196</v>
+        <v>2.894958499480917</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.6429349999999999</v>
+        <v>-25.1196228</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1205961300622868</v>
+        <v>11.58173588351275</v>
       </c>
     </row>
     <row r="27">
@@ -1450,7 +1442,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1463,11 +1455,15 @@
           <t>Event 2</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>1.83848</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.1884796048733125</v>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1488,7 +1484,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1530,7 +1526,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1544,16 +1540,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>70.40000000000001</v>
+        <v>34.4</v>
       </c>
       <c r="F29" t="n">
-        <v>1.356465996625054</v>
+        <v>1.019803902718557</v>
       </c>
       <c r="G29" t="n">
-        <v>16</v>
+        <v>96.8</v>
       </c>
       <c r="H29" t="n">
-        <v>1.095445115010332</v>
+        <v>1.720465053408525</v>
       </c>
     </row>
     <row r="30">
@@ -1564,7 +1560,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1606,7 +1602,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1648,7 +1644,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1662,16 +1658,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>78.40000000000001</v>
+        <v>30.4</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8</v>
+        <v>1.959591794226543</v>
       </c>
       <c r="G32" t="n">
-        <v>15.8</v>
+        <v>97.59999999999999</v>
       </c>
       <c r="H32" t="n">
-        <v>0.7483314773547883</v>
+        <v>0.4898979485566356</v>
       </c>
     </row>
     <row r="33">
@@ -1682,7 +1678,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1724,7 +1720,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1766,7 +1762,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1780,16 +1776,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>80.40000000000001</v>
+        <v>31.4</v>
       </c>
       <c r="F35" t="n">
-        <v>0.8</v>
+        <v>2.154065922853801</v>
       </c>
       <c r="G35" t="n">
-        <v>15.6</v>
+        <v>99.59999999999999</v>
       </c>
       <c r="H35" t="n">
-        <v>1.019803902718557</v>
+        <v>2.33238075793812</v>
       </c>
     </row>
     <row r="36">
@@ -1800,7 +1796,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1842,7 +1838,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1884,7 +1880,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1897,21 +1893,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E38" t="n">
+        <v>109.8</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1.16619037896906</v>
       </c>
       <c r="G38" t="n">
-        <v>77</v>
+        <v>187.6</v>
       </c>
       <c r="H38" t="n">
-        <v>0.6324555320336759</v>
+        <v>3.006659275674582</v>
       </c>
     </row>
     <row r="39">
@@ -1922,7 +1914,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1964,7 +1956,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2006,7 +1998,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2019,21 +2011,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E41" t="n">
+        <v>108.6</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2.33238075793812</v>
       </c>
       <c r="G41" t="n">
-        <v>78.40000000000001</v>
+        <v>190.4</v>
       </c>
       <c r="H41" t="n">
-        <v>0.8</v>
+        <v>4.409081537009721</v>
       </c>
     </row>
     <row r="42">
@@ -2044,7 +2032,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2086,7 +2074,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2128,7 +2116,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2141,21 +2129,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E44" t="n">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="F44" t="n">
+        <v>12.73734666247253</v>
       </c>
       <c r="G44" t="n">
-        <v>76</v>
+        <v>162.6</v>
       </c>
       <c r="H44" t="n">
-        <v>1.095445115010332</v>
+        <v>36.61475112574166</v>
       </c>
     </row>
     <row r="45">
@@ -2166,7 +2150,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2208,7 +2192,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2250,7 +2234,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2264,16 +2248,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>21.2</v>
+        <v>51.6</v>
       </c>
       <c r="F47" t="n">
-        <v>1.720465053408525</v>
+        <v>19.34528366295</v>
       </c>
       <c r="G47" t="n">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="H47" t="n">
-        <v>22</v>
+        <v>60.44501633716381</v>
       </c>
     </row>
     <row r="48">
@@ -2284,7 +2268,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2297,11 +2281,15 @@
           <t>Event 2</t>
         </is>
       </c>
-      <c r="E48" t="n">
-        <v>87</v>
-      </c>
-      <c r="F48" t="n">
-        <v>1.095445115010332</v>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2322,7 +2310,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2364,7 +2352,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2378,16 +2366,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>18.8</v>
+        <v>17.2</v>
       </c>
       <c r="F50" t="n">
-        <v>0.7483314773547883</v>
+        <v>3.124099870362662</v>
       </c>
       <c r="G50" t="n">
-        <v>8.800000000000001</v>
+        <v>67.2</v>
       </c>
       <c r="H50" t="n">
-        <v>0.4</v>
+        <v>1.32664991614216</v>
       </c>
     </row>
     <row r="51">
@@ -2398,7 +2386,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2412,16 +2400,16 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>88.59999999999999</v>
+        <v>115.6</v>
       </c>
       <c r="F51" t="n">
-        <v>0.4898979485566356</v>
+        <v>4.223742416388575</v>
       </c>
       <c r="G51" t="n">
-        <v>68.40000000000001</v>
+        <v>189.2</v>
       </c>
       <c r="H51" t="n">
-        <v>1.356465996625054</v>
+        <v>3.487119154832539</v>
       </c>
     </row>
     <row r="52">
@@ -2432,7 +2420,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2474,7 +2462,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2488,16 +2476,16 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>20.8</v>
+        <v>61.6</v>
       </c>
       <c r="F53" t="n">
-        <v>1.16619037896906</v>
+        <v>4.963869458396342</v>
       </c>
       <c r="G53" t="n">
-        <v>31.2</v>
+        <v>162</v>
       </c>
       <c r="H53" t="n">
-        <v>27.60724542579357</v>
+        <v>20.01999000998752</v>
       </c>
     </row>
     <row r="54">
@@ -2508,7 +2496,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2521,11 +2509,15 @@
           <t>Event 2</t>
         </is>
       </c>
-      <c r="E54" t="n">
-        <v>88.8</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.7483314773547882</v>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2546,7 +2538,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2588,7 +2580,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2602,16 +2594,16 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>69.70297029702969</v>
+        <v>16.45933014</v>
       </c>
       <c r="F56" t="n">
-        <v>1.343035640222822</v>
+        <v>0.4879444515494543</v>
       </c>
       <c r="G56" t="n">
-        <v>15.84158415841584</v>
+        <v>46.31578947000001</v>
       </c>
       <c r="H56" t="n">
-        <v>1.084599123772606</v>
+        <v>0.823189021592818</v>
       </c>
     </row>
     <row r="57">
@@ -2622,7 +2614,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2664,7 +2656,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2706,7 +2698,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2720,16 +2712,16 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>77.62376237623762</v>
+        <v>14.545454548</v>
       </c>
       <c r="F59" t="n">
-        <v>0.79207920792079</v>
+        <v>0.9376037265583655</v>
       </c>
       <c r="G59" t="n">
-        <v>15.64356435643564</v>
+        <v>46.69856459</v>
       </c>
       <c r="H59" t="n">
-        <v>0.7409222548067217</v>
+        <v>0.234400932558148</v>
       </c>
     </row>
     <row r="60">
@@ -2740,7 +2732,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2782,7 +2774,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2824,7 +2816,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2838,16 +2830,16 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>79.60396039603961</v>
+        <v>15.023923444</v>
       </c>
       <c r="F62" t="n">
-        <v>0.7920792079207963</v>
+        <v>1.030653548178655</v>
       </c>
       <c r="G62" t="n">
-        <v>15.44554455445545</v>
+        <v>47.65550239</v>
       </c>
       <c r="H62" t="n">
-        <v>1.009706834374809</v>
+        <v>1.11597165563182</v>
       </c>
     </row>
     <row r="63">
@@ -2858,7 +2850,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2900,7 +2892,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2942,7 +2934,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2955,21 +2947,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E65" t="n">
+        <v>52.53588516999999</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.5579858278159094</v>
       </c>
       <c r="G65" t="n">
-        <v>76.23762376237624</v>
+        <v>89.76076555</v>
       </c>
       <c r="H65" t="n">
-        <v>0.6261935960729492</v>
+        <v>1.43859295630681</v>
       </c>
     </row>
     <row r="66">
@@ -2980,7 +2968,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3022,7 +3010,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3064,7 +3052,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3077,21 +3065,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E68" t="n">
+        <v>51.96172249</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1.115971655631818</v>
       </c>
       <c r="G68" t="n">
-        <v>77.62376237623762</v>
+        <v>91.10047847</v>
       </c>
       <c r="H68" t="n">
-        <v>0.79207920792079</v>
+        <v>2.109608393023349</v>
       </c>
     </row>
     <row r="69">
@@ -3102,7 +3086,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3144,7 +3128,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3186,7 +3170,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3199,21 +3183,17 @@
           <t>Event 1</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="E71" t="n">
+        <v>47.559808612</v>
+      </c>
+      <c r="F71" t="n">
+        <v>6.094424242523628</v>
       </c>
       <c r="G71" t="n">
-        <v>75.24752475247524</v>
+        <v>77.799043062</v>
       </c>
       <c r="H71" t="n">
-        <v>1.084599123772608</v>
+        <v>17.51901967586587</v>
       </c>
     </row>
     <row r="72">
@@ -3224,7 +3204,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3266,7 +3246,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3308,7 +3288,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3322,16 +3302,16 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>20.99009900990099</v>
+        <v>24.6889952148</v>
       </c>
       <c r="F74" t="n">
-        <v>1.703430745949035</v>
+        <v>9.256116584822125</v>
       </c>
       <c r="G74" t="n">
-        <v>18.81188118811881</v>
+        <v>63.157894738</v>
       </c>
       <c r="H74" t="n">
-        <v>21.78217821782178</v>
+        <v>28.92106044814125</v>
       </c>
     </row>
     <row r="75">
@@ -3342,7 +3322,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3355,11 +3335,15 @@
           <t>Event 2</t>
         </is>
       </c>
-      <c r="E75" t="n">
-        <v>86.13861386138613</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1.084599123772608</v>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3380,7 +3364,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3422,7 +3406,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3436,16 +3420,16 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>18.61386138613862</v>
+        <v>8.229665072</v>
       </c>
       <c r="F77" t="n">
-        <v>0.7409222548067217</v>
+        <v>1.49478462705416</v>
       </c>
       <c r="G77" t="n">
-        <v>8.712871287128712</v>
+        <v>32.15311005</v>
       </c>
       <c r="H77" t="n">
-        <v>0.3960396039603957</v>
+        <v>0.6347607260616329</v>
       </c>
     </row>
     <row r="78">
@@ -3456,7 +3440,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3470,16 +3454,16 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>87.72277227722773</v>
+        <v>55.311004786</v>
       </c>
       <c r="F78" t="n">
-        <v>0.4850474738184498</v>
+        <v>2.02092938321235</v>
       </c>
       <c r="G78" t="n">
-        <v>67.72277227722773</v>
+        <v>90.52631578999998</v>
       </c>
       <c r="H78" t="n">
-        <v>1.343035640222822</v>
+        <v>1.668478066181654</v>
       </c>
     </row>
     <row r="79">
@@ -3490,7 +3474,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3532,7 +3516,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3546,16 +3530,16 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>20.59405940594059</v>
+        <v>29.47368421</v>
       </c>
       <c r="F80" t="n">
-        <v>1.154643939573328</v>
+        <v>2.375057159502493</v>
       </c>
       <c r="G80" t="n">
-        <v>30.89108910891089</v>
+        <v>77.51196172</v>
       </c>
       <c r="H80" t="n">
-        <v>27.33390636217186</v>
+        <v>9.578942589798002</v>
       </c>
     </row>
     <row r="81">
@@ -3566,7 +3550,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3579,11 +3563,15 @@
           <t>Event 2</t>
         </is>
       </c>
-      <c r="E81" t="n">
-        <v>87.92079207920793</v>
-      </c>
-      <c r="F81" t="n">
-        <v>0.740922254806719</v>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3604,7 +3592,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3707,7 +3695,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3741,7 +3729,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3783,7 +3771,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3825,7 +3813,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3859,7 +3847,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3901,7 +3889,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3943,7 +3931,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -3977,7 +3965,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4019,7 +4007,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4061,7 +4049,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4099,7 +4087,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -4141,7 +4129,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -4183,7 +4171,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -4221,7 +4209,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -4263,7 +4251,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -4305,7 +4293,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -4343,7 +4331,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -4385,7 +4373,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -4427,7 +4415,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -4461,7 +4449,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -4503,7 +4491,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -4545,7 +4533,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -4579,7 +4567,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -4613,7 +4601,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -4655,7 +4643,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4689,7 +4677,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4731,7 +4719,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -4773,7 +4761,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -4807,7 +4795,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -4849,7 +4837,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -4891,7 +4879,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -4925,7 +4913,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -4967,7 +4955,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -5009,7 +4997,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -5043,7 +5031,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -5085,7 +5073,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -5127,7 +5115,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -5165,7 +5153,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -5207,7 +5195,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -5249,7 +5237,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -5287,7 +5275,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -5329,7 +5317,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -5371,7 +5359,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -5409,7 +5397,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -5451,7 +5439,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -5493,7 +5481,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -5527,7 +5515,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -5569,7 +5557,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -5611,7 +5599,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -5645,7 +5633,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -5679,7 +5667,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -5721,7 +5709,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -5755,7 +5743,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -5797,7 +5785,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -5839,7 +5827,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -5853,16 +5841,16 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>74.05940594059408</v>
+        <v>74.05940593799998</v>
       </c>
       <c r="F56" t="n">
-        <v>1.455142421455353</v>
+        <v>1.45514242160087</v>
       </c>
       <c r="G56" t="n">
-        <v>12.67326732673267</v>
+        <v>12.6732673278</v>
       </c>
       <c r="H56" t="n">
-        <v>3.337089019079746</v>
+        <v>3.337089019757622</v>
       </c>
     </row>
     <row r="57">
@@ -5873,7 +5861,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -5915,7 +5903,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -5957,7 +5945,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -5971,16 +5959,16 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>75.84158415841584</v>
+        <v>75.841584156</v>
       </c>
       <c r="F59" t="n">
-        <v>0.7920792079207964</v>
+        <v>0.792079208000002</v>
       </c>
       <c r="G59" t="n">
-        <v>15.44554455445545</v>
+        <v>15.445544556</v>
       </c>
       <c r="H59" t="n">
-        <v>0.7920792079207928</v>
+        <v>0.7920792080000004</v>
       </c>
     </row>
     <row r="60">
@@ -5991,7 +5979,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -6033,7 +6021,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -6075,7 +6063,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -6089,16 +6077,16 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>78.61386138613861</v>
+        <v>78.613861384</v>
       </c>
       <c r="F62" t="n">
-        <v>1.009706834374811</v>
+        <v>1.00970683447578</v>
       </c>
       <c r="G62" t="n">
-        <v>13.66336633663366</v>
+        <v>13.663366338</v>
       </c>
       <c r="H62" t="n">
-        <v>1.154643939573327</v>
+        <v>1.154643939688791</v>
       </c>
     </row>
     <row r="63">
@@ -6109,7 +6097,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -6151,7 +6139,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>LeftAnkleAngle_X</t>
+          <t>Right_Ankle_Angle_X</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -6193,7 +6181,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -6217,10 +6205,10 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>77.22772277227722</v>
+        <v>77.22772277000001</v>
       </c>
       <c r="H65" t="n">
-        <v>1.400211447894154</v>
+        <v>1.400211448034175</v>
       </c>
     </row>
     <row r="66">
@@ -6231,7 +6219,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -6273,7 +6261,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -6315,7 +6303,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -6339,10 +6327,10 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>77.62376237623764</v>
+        <v>77.62376237399999</v>
       </c>
       <c r="H68" t="n">
-        <v>0.4850474738184498</v>
+        <v>0.4850474738669531</v>
       </c>
     </row>
     <row r="69">
@@ -6353,7 +6341,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -6395,7 +6383,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -6437,7 +6425,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -6461,10 +6449,10 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>79.20792079207922</v>
+        <v>79.20792079</v>
       </c>
       <c r="H71" t="n">
-        <v>0.6261935960729492</v>
+        <v>0.6261935961355667</v>
       </c>
     </row>
     <row r="72">
@@ -6475,7 +6463,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -6517,7 +6505,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>LeftAnkleMoment_X</t>
+          <t>Right_Ankle_Moment_X</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -6559,7 +6547,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -6573,16 +6561,16 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>32.27722772277227</v>
+        <v>32.277227724</v>
       </c>
       <c r="F74" t="n">
-        <v>26.95979790117625</v>
+        <v>26.95979789987655</v>
       </c>
       <c r="G74" t="n">
-        <v>36.83168316831682</v>
+        <v>36.8316831676</v>
       </c>
       <c r="H74" t="n">
-        <v>23.1132458794691</v>
+        <v>23.11324587844258</v>
       </c>
     </row>
     <row r="75">
@@ -6593,7 +6581,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -6635,7 +6623,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -6677,7 +6665,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -6691,16 +6679,16 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>19.20792079207921</v>
+        <v>19.207920794</v>
       </c>
       <c r="F77" t="n">
-        <v>1.00970683437481</v>
+        <v>1.00970683447578</v>
       </c>
       <c r="G77" t="n">
-        <v>8.514851485148515</v>
+        <v>8.514851484999999</v>
       </c>
       <c r="H77" t="n">
-        <v>0.4850474738184506</v>
+        <v>0.4850474738669557</v>
       </c>
     </row>
     <row r="78">
@@ -6711,7 +6699,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -6725,16 +6713,16 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>87.92079207920793</v>
+        <v>87.92079207800001</v>
       </c>
       <c r="F78" t="n">
-        <v>0.3960396039603949</v>
+        <v>0.3960396039999978</v>
       </c>
       <c r="G78" t="n">
-        <v>65.94059405940595</v>
+        <v>65.94059405599999</v>
       </c>
       <c r="H78" t="n">
-        <v>0.4850474738184498</v>
+        <v>0.4850474738669601</v>
       </c>
     </row>
     <row r="79">
@@ -6745,7 +6733,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -6787,7 +6775,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -6801,16 +6789,16 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>32.47524752475248</v>
+        <v>32.475247526</v>
       </c>
       <c r="F80" t="n">
-        <v>28.32721543326363</v>
+        <v>28.32721543209782</v>
       </c>
       <c r="G80" t="n">
-        <v>56.83168316831683</v>
+        <v>56.83168316579999</v>
       </c>
       <c r="H80" t="n">
-        <v>24.99759815930218</v>
+        <v>24.99759815820872</v>
       </c>
     </row>
     <row r="81">
@@ -6821,7 +6809,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -6863,7 +6851,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>LeftAnklePower_X</t>
+          <t>Right_Ankle_Power_X</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">

</xml_diff>